<commit_message>
Combined commit no 2 and commit no 3 to a single commit Commit No 2 - Files modified Commit No 3 - Modified both files even further
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Projects\test-repo\MergeConflict-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DBC084-D156-48B5-BB49-EACA119531D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B2BACA-063D-4382-BC9F-94567A253945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,9 +27,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>this is in first commit</t>
+  </si>
+  <si>
+    <t>this is my second commit</t>
+  </si>
+  <si>
+    <t>this is also part of second commit</t>
+  </si>
+  <si>
+    <t>added this in 3rd commit</t>
+  </si>
+  <si>
+    <t>this is part of third commit</t>
   </si>
 </sst>
 </file>
@@ -345,6 +359,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13702635-E6B3-4B31-8F84-7DB407FAE0D6}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666A9186-04DB-4A5A-B186-315BF4FFEC2A}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -355,7 +419,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>